<commit_message>
changed a few cells' syntax
</commit_message>
<xml_diff>
--- a/expense-report-review-calculator.xlsx
+++ b/expense-report-review-calculator.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\hihipy\coding-workspace\useful-job-tools\Expense-Report-Review-Calculator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\hihipy\coding-workspace\useful-job-tools\expense-report-review-calculator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D324471-6221-4555-9714-432211272911}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F4CB769-EE85-4765-9622-4F8DDE0878B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{9EB0749C-90DE-4314-8D7D-2707C09E549F}"/>
   </bookViews>
@@ -72,9 +72,6 @@
     <t>Notes</t>
   </si>
   <si>
-    <t># Days &gt;60</t>
-  </si>
-  <si>
     <t>EXP Submission Date</t>
   </si>
   <si>
@@ -94,6 +91,9 @@
   </si>
   <si>
     <t>Institution’s Upper Limit of Days After Expense was Paid or Incurred</t>
+  </si>
+  <si>
+    <t># Days &gt; Institution’s Upper Limit of Days After Expense was Paid or Incurred</t>
   </si>
 </sst>
 </file>
@@ -360,6 +360,15 @@
     <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="1" fontId="7" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -383,15 +392,6 @@
     </xf>
     <xf numFmtId="1" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -544,7 +544,7 @@
     <tableColumn id="2" xr3:uid="{847CC89E-9549-4D2E-A289-5BA063AB0767}" name="Date of Expense" dataDxfId="3"/>
     <tableColumn id="3" xr3:uid="{F7577957-29D5-4CA4-BB08-E2352CA02DC2}" name="USD" dataDxfId="2"/>
     <tableColumn id="4" xr3:uid="{86E9BD60-88D4-4DBA-8863-1E4B3672BE98}" name="Notes" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{94442348-A842-4B9E-8438-186F22B4E931}" name="# Days &gt;60" dataDxfId="0">
+    <tableColumn id="7" xr3:uid="{94442348-A842-4B9E-8438-186F22B4E931}" name="# Days &gt; Institution’s Upper Limit of Days After Expense was Paid or Incurred" dataDxfId="0">
       <calculatedColumnFormula array="1">_xlfn.IFS(OR(ISERROR(B$3-B9), ISBLANK(B9), ISBLANK(C9)), "Enter Data in both Row 1 &amp; Starting at Row 8", B$3&gt;B9, B$3-B9, TRUE, "N/A")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -853,7 +853,7 @@
   <dimension ref="A1:I59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="H15" sqref="H14:H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -862,69 +862,69 @@
     <col min="2" max="2" width="32.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28.42578125" style="4" customWidth="1"/>
     <col min="4" max="4" width="38.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="58.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="96.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" style="2" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
+      <c r="A1" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
       <c r="D1" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="25"/>
+      <c r="A2" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="27"/>
+      <c r="C2" s="28"/>
       <c r="D2" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="str">
+      <c r="A3" s="18" t="str">
         <f>B2&amp;" Days Ago Date"</f>
         <v xml:space="preserve"> Days Ago Date</v>
       </c>
-      <c r="B3" s="22" t="str">
+      <c r="B3" s="25" t="str">
         <f>IF(ISBLANK(B1), "Enter EXP Submission Date at Row 1", B1-B2)</f>
         <v>Enter EXP Submission Date at Row 1</v>
       </c>
-      <c r="C3" s="23"/>
+      <c r="C3" s="26"/>
       <c r="D3" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="20" t="str">
+      <c r="B4" s="23" t="str">
         <f>IF(OR(ISBLANK(B9), ISBLANK(C9), ISBLANK(B1)),"Enter Data Starting in Rows 1 &amp; 8", SUM(Table1[USD]))</f>
         <v>Enter Data Starting in Rows 1 &amp; 8</v>
       </c>
-      <c r="C4" s="20"/>
+      <c r="C4" s="23"/>
       <c r="D4" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A5" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="18" t="str">
+      <c r="A5" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="21" t="str">
         <f>IF(OR(ISBLANK(B9), ISBLANK(C9), ISBLANK(B1)),"Enter Data Starting in Rows 1 &amp; 8", COUNTA(Table1[Date of Expense]))</f>
         <v>Enter Data Starting in Rows 1 &amp; 8</v>
       </c>
-      <c r="C5" s="19"/>
+      <c r="C5" s="22"/>
       <c r="D5" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -935,19 +935,19 @@
     </row>
     <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="6" t="s">
         <v>8</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -955,7 +955,7 @@
         <v>0</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>1</v>
@@ -964,7 +964,7 @@
         <v>3</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
readme additions and small file changes.
</commit_message>
<xml_diff>
--- a/expense-report-review-calculator.xlsx
+++ b/expense-report-review-calculator.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\hihipy\coding-workspace\useful-job-tools\expense-report-review-calculator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bd6fd30e1a3dec7d/coding-workspace/useful-job-tools/expense-report-review-calculator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A6251C3-12AF-46A3-9EFF-2310612E2BA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="13_ncr:1_{2A6251C3-12AF-46A3-9EFF-2310612E2BA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{66594A1F-759F-EF4D-B1BC-060FA07E1A1A}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{9EB0749C-90DE-4314-8D7D-2707C09E549F}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="24140" windowHeight="26800" xr2:uid="{9EB0749C-90DE-4314-8D7D-2707C09E549F}"/>
   </bookViews>
   <sheets>
     <sheet name="Calculator" sheetId="1" r:id="rId1"/>
@@ -381,17 +381,17 @@
     <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="7" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -401,21 +401,6 @@
     <cellStyle name="Note" xfId="3" builtinId="10"/>
   </cellStyles>
   <dxfs count="8">
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Consolas"/>
-        <family val="3"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -509,6 +494,21 @@
         <family val="3"/>
         <scheme val="none"/>
       </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -537,14 +537,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D8C5EBB0-BFD2-43B5-9865-41A9B951F4B6}" name="Table1" displayName="Table1" ref="A8:E55" totalsRowShown="0" headerRowDxfId="6" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D8C5EBB0-BFD2-43B5-9865-41A9B951F4B6}" name="Table1" displayName="Table1" ref="A8:E55" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
   <autoFilter ref="A8:E55" xr:uid="{FC060CE5-3EF0-4040-92D1-4AED472000A2}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{931DCCE9-E379-43B2-91F7-D4E1BD90235B}" name="Page #" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{847CC89E-9549-4D2E-A289-5BA063AB0767}" name="Date of Expense" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{F7577957-29D5-4CA4-BB08-E2352CA02DC2}" name="Currency Amount" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{86E9BD60-88D4-4DBA-8863-1E4B3672BE98}" name="Notes" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{94442348-A842-4B9E-8438-186F22B4E931}" name="# Days &gt; Institution’s Upper Limit of Days After Expense was Paid or Incurred" dataDxfId="1">
+    <tableColumn id="1" xr3:uid="{931DCCE9-E379-43B2-91F7-D4E1BD90235B}" name="Page #" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{847CC89E-9549-4D2E-A289-5BA063AB0767}" name="Date of Expense" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{F7577957-29D5-4CA4-BB08-E2352CA02DC2}" name="Currency Amount" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{86E9BD60-88D4-4DBA-8863-1E4B3672BE98}" name="Notes" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{94442348-A842-4B9E-8438-186F22B4E931}" name="# Days &gt; Institution’s Upper Limit of Days After Expense was Paid or Incurred" dataDxfId="0">
       <calculatedColumnFormula array="1">_xlfn.IFS(OR(ISERROR(B$3-B9), ISBLANK(B9), ISBLANK(C9)), "Enter Data in both Row 1 &amp; Starting at Row 8", B$3&gt;B9, B$3-B9, TRUE, "N/A")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -853,21 +853,21 @@
   <dimension ref="A1:I59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.42578125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="38.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="26.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.5" style="4" customWidth="1"/>
+    <col min="4" max="4" width="38.6640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="53" style="2" customWidth="1"/>
     <col min="6" max="6" width="9" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="2"/>
+    <col min="7" max="16384" width="9.1640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="23" x14ac:dyDescent="0.2">
       <c r="A1" s="18" t="s">
         <v>2</v>
       </c>
@@ -877,31 +877,31 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A2" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="28"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="26"/>
       <c r="D2" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="18" t="str">
         <f>B2&amp;" Days Ago Date"</f>
         <v xml:space="preserve"> Days Ago Date</v>
       </c>
-      <c r="B3" s="25" t="str">
-        <f>IF(ISBLANK(B1), "Enter EXP Submission Date at Row 1", B1-B2)</f>
-        <v>Enter EXP Submission Date at Row 1</v>
-      </c>
-      <c r="C3" s="26"/>
+      <c r="B3" s="27" t="str">
+        <f>IF(ISBLANK(B1), "Enter EXP Submission Date at Row 1 &amp; Institution’s Upper Limit of Days After Expense was Paid or Incurred at Row 2", B1-B2)</f>
+        <v>Enter EXP Submission Date at Row 1 &amp; Institution’s Upper Limit of Days After Expense was Paid or Incurred at Row 2</v>
+      </c>
+      <c r="C3" s="28"/>
       <c r="D3" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="23" x14ac:dyDescent="0.2">
       <c r="A4" s="19" t="s">
         <v>11</v>
       </c>
@@ -914,7 +914,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="23" x14ac:dyDescent="0.2">
       <c r="A5" s="18" t="s">
         <v>4</v>
       </c>
@@ -927,13 +927,13 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="7"/>
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
       <c r="D6" s="10"/>
     </row>
-    <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
@@ -950,7 +950,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
@@ -967,17 +967,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="11"/>
       <c r="B9" s="13"/>
       <c r="C9" s="17"/>
       <c r="D9" s="11"/>
       <c r="E9" s="15" t="str" cm="1">
-        <f t="array" ref="E9">_xlfn.IFS(OR(ISERROR(B$3-B9), ISBLANK(B9), ISBLANK(C9)), "Enter Data in Row 1 and Starting on Row 9", B$3&gt;B9, B$3-B9, TRUE, "N/A")</f>
-        <v>Enter Data in Row 1 and Starting on Row 9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <f t="array" ref="E9">_xlfn.IFS(OR(ISERROR(B$3-B9), ISBLANK(B9), ISBLANK(C9)), "Enter Data in Row 1, Row 2,  &amp; Starting on Row 9", B$3&gt;B9, B$3-B9, TRUE, "N/A")</f>
+        <v>Enter Data in Row 1, Row 2,  &amp; Starting on Row 9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="11"/>
       <c r="B10" s="13"/>
       <c r="C10" s="17"/>
@@ -988,7 +988,7 @@
       </c>
       <c r="I10" s="3"/>
     </row>
-    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" s="11"/>
       <c r="B11" s="13"/>
       <c r="C11" s="17"/>
@@ -998,7 +998,7 @@
         <v>Enter Data in 'Date of Expense' &amp; 'Currency Amount' as Needed</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="11"/>
       <c r="B12" s="13"/>
       <c r="C12" s="17"/>
@@ -1008,7 +1008,7 @@
         <v>Enter Data in 'Date of Expense' &amp; 'Currency Amount' as Needed</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" s="11"/>
       <c r="B13" s="13"/>
       <c r="C13" s="17"/>
@@ -1018,7 +1018,7 @@
         <v>Enter Data in 'Date of Expense' &amp; 'Currency Amount' as Needed</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A14" s="11"/>
       <c r="B14" s="13"/>
       <c r="C14" s="17"/>
@@ -1028,7 +1028,7 @@
         <v>Enter Data in 'Date of Expense' &amp; 'Currency Amount' as Needed</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" s="11"/>
       <c r="B15" s="13"/>
       <c r="C15" s="17"/>
@@ -1038,7 +1038,7 @@
         <v>Enter Data in 'Date of Expense' &amp; 'Currency Amount' as Needed</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A16" s="11"/>
       <c r="B16" s="13"/>
       <c r="C16" s="17"/>
@@ -1048,7 +1048,7 @@
         <v>Enter Data in 'Date of Expense' &amp; 'Currency Amount' as Needed</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="11"/>
       <c r="B17" s="13"/>
       <c r="C17" s="17"/>
@@ -1058,7 +1058,7 @@
         <v>Enter Data in 'Date of Expense' &amp; 'Currency Amount' as Needed</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A18" s="11"/>
       <c r="B18" s="13"/>
       <c r="C18" s="17"/>
@@ -1068,7 +1068,7 @@
         <v>Enter Data in 'Date of Expense' &amp; 'Currency Amount' as Needed</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" s="11"/>
       <c r="B19" s="13"/>
       <c r="C19" s="17"/>
@@ -1078,7 +1078,7 @@
         <v>Enter Data in 'Date of Expense' &amp; 'Currency Amount' as Needed</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A20" s="11"/>
       <c r="B20" s="13"/>
       <c r="C20" s="17"/>
@@ -1088,7 +1088,7 @@
         <v>Enter Data in 'Date of Expense' &amp; 'Currency Amount' as Needed</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A21" s="11"/>
       <c r="B21" s="13"/>
       <c r="C21" s="17"/>
@@ -1098,7 +1098,7 @@
         <v>Enter Data in 'Date of Expense' &amp; 'Currency Amount' as Needed</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A22" s="11"/>
       <c r="B22" s="13"/>
       <c r="C22" s="17"/>
@@ -1108,7 +1108,7 @@
         <v>Enter Data in 'Date of Expense' &amp; 'Currency Amount' as Needed</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A23" s="11"/>
       <c r="B23" s="13"/>
       <c r="C23" s="17"/>
@@ -1118,7 +1118,7 @@
         <v>Enter Data in 'Date of Expense' &amp; 'Currency Amount' as Needed</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A24" s="11"/>
       <c r="B24" s="13"/>
       <c r="C24" s="17"/>
@@ -1128,7 +1128,7 @@
         <v>Enter Data in 'Date of Expense' &amp; 'Currency Amount' as Needed</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A25" s="11"/>
       <c r="B25" s="13"/>
       <c r="C25" s="17"/>
@@ -1138,7 +1138,7 @@
         <v>Enter Data in 'Date of Expense' &amp; 'Currency Amount' as Needed</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A26" s="11"/>
       <c r="B26" s="13"/>
       <c r="C26" s="17"/>
@@ -1148,7 +1148,7 @@
         <v>Enter Data in 'Date of Expense' &amp; 'Currency Amount' as Needed</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A27" s="11"/>
       <c r="B27" s="13"/>
       <c r="C27" s="17"/>
@@ -1158,7 +1158,7 @@
         <v>Enter Data in 'Date of Expense' &amp; 'Currency Amount' as Needed</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A28" s="11"/>
       <c r="B28" s="13"/>
       <c r="C28" s="17"/>
@@ -1168,7 +1168,7 @@
         <v>Enter Data in 'Date of Expense' &amp; 'Currency Amount' as Needed</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A29" s="11"/>
       <c r="B29" s="13"/>
       <c r="C29" s="17"/>
@@ -1178,7 +1178,7 @@
         <v>Enter Data in 'Date of Expense' &amp; 'Currency Amount' as Needed</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A30" s="11"/>
       <c r="B30" s="13"/>
       <c r="C30" s="17"/>
@@ -1188,7 +1188,7 @@
         <v>Enter Data in 'Date of Expense' &amp; 'Currency Amount' as Needed</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A31" s="11"/>
       <c r="B31" s="13"/>
       <c r="C31" s="17"/>
@@ -1198,7 +1198,7 @@
         <v>Enter Data in 'Date of Expense' &amp; 'Currency Amount' as Needed</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A32" s="11"/>
       <c r="B32" s="13"/>
       <c r="C32" s="17"/>
@@ -1208,7 +1208,7 @@
         <v>Enter Data in 'Date of Expense' &amp; 'Currency Amount' as Needed</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A33" s="11"/>
       <c r="B33" s="13"/>
       <c r="C33" s="17"/>
@@ -1218,7 +1218,7 @@
         <v>Enter Data in 'Date of Expense' &amp; 'Currency Amount' as Needed</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A34" s="11"/>
       <c r="B34" s="13"/>
       <c r="C34" s="17"/>
@@ -1228,7 +1228,7 @@
         <v>Enter Data in 'Date of Expense' &amp; 'Currency Amount' as Needed</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A35" s="11"/>
       <c r="B35" s="13"/>
       <c r="C35" s="17"/>
@@ -1238,7 +1238,7 @@
         <v>Enter Data in 'Date of Expense' &amp; 'Currency Amount' as Needed</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A36" s="11"/>
       <c r="B36" s="13"/>
       <c r="C36" s="17"/>
@@ -1248,7 +1248,7 @@
         <v>Enter Data in 'Date of Expense' &amp; 'Currency Amount' as Needed</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A37" s="11"/>
       <c r="B37" s="13"/>
       <c r="C37" s="17"/>
@@ -1258,7 +1258,7 @@
         <v>Enter Data in 'Date of Expense' &amp; 'Currency Amount' as Needed</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A38" s="11"/>
       <c r="B38" s="13"/>
       <c r="C38" s="17"/>
@@ -1268,7 +1268,7 @@
         <v>Enter Data in 'Date of Expense' &amp; 'Currency Amount' as Needed</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A39" s="11"/>
       <c r="B39" s="13"/>
       <c r="C39" s="17"/>
@@ -1278,7 +1278,7 @@
         <v>Enter Data in 'Date of Expense' &amp; 'Currency Amount' as Needed</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A40" s="11"/>
       <c r="B40" s="13"/>
       <c r="C40" s="17"/>
@@ -1288,7 +1288,7 @@
         <v>Enter Data in 'Date of Expense' &amp; 'Currency Amount' as Needed</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A41" s="11"/>
       <c r="B41" s="13"/>
       <c r="C41" s="17"/>
@@ -1298,7 +1298,7 @@
         <v>Enter Data in 'Date of Expense' &amp; 'Currency Amount' as Needed</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A42" s="11"/>
       <c r="B42" s="13"/>
       <c r="C42" s="17"/>
@@ -1308,7 +1308,7 @@
         <v>Enter Data in 'Date of Expense' &amp; 'Currency Amount' as Needed</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A43" s="11"/>
       <c r="B43" s="13"/>
       <c r="C43" s="17"/>
@@ -1318,7 +1318,7 @@
         <v>Enter Data in 'Date of Expense' &amp; 'Currency Amount' as Needed</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A44" s="11"/>
       <c r="B44" s="13"/>
       <c r="C44" s="17"/>
@@ -1328,7 +1328,7 @@
         <v>Enter Data in 'Date of Expense' &amp; 'Currency Amount' as Needed</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A45" s="11"/>
       <c r="B45" s="13"/>
       <c r="C45" s="17"/>
@@ -1338,7 +1338,7 @@
         <v>Enter Data in 'Date of Expense' &amp; 'Currency Amount' as Needed</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A46" s="11"/>
       <c r="B46" s="13"/>
       <c r="C46" s="17"/>
@@ -1348,7 +1348,7 @@
         <v>Enter Data in 'Date of Expense' &amp; 'Currency Amount' as Needed</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A47" s="11"/>
       <c r="B47" s="13"/>
       <c r="C47" s="17"/>
@@ -1358,7 +1358,7 @@
         <v>Enter Data in 'Date of Expense' &amp; 'Currency Amount' as Needed</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A48" s="11"/>
       <c r="B48" s="13"/>
       <c r="C48" s="17"/>
@@ -1368,7 +1368,7 @@
         <v>Enter Data in 'Date of Expense' &amp; 'Currency Amount' as Needed</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A49" s="11"/>
       <c r="B49" s="13"/>
       <c r="C49" s="17"/>
@@ -1378,7 +1378,7 @@
         <v>Enter Data in 'Date of Expense' &amp; 'Currency Amount' as Needed</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A50" s="11"/>
       <c r="B50" s="13"/>
       <c r="C50" s="17"/>
@@ -1388,7 +1388,7 @@
         <v>Enter Data in 'Date of Expense' &amp; 'Currency Amount' as Needed</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A51" s="11"/>
       <c r="B51" s="13"/>
       <c r="C51" s="17"/>
@@ -1398,7 +1398,7 @@
         <v>Enter Data in 'Date of Expense' &amp; 'Currency Amount' as Needed</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A52" s="11"/>
       <c r="B52" s="13"/>
       <c r="C52" s="17"/>
@@ -1408,7 +1408,7 @@
         <v>Enter Data in 'Date of Expense' &amp; 'Currency Amount' as Needed</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A53" s="11"/>
       <c r="B53" s="13"/>
       <c r="C53" s="17"/>
@@ -1418,7 +1418,7 @@
         <v>Enter Data in 'Date of Expense' &amp; 'Currency Amount' as Needed</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A54" s="11"/>
       <c r="B54" s="13"/>
       <c r="C54" s="17"/>
@@ -1428,7 +1428,7 @@
         <v>Enter Data in 'Date of Expense' &amp; 'Currency Amount' as Needed</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A55" s="11"/>
       <c r="B55" s="13"/>
       <c r="C55" s="17"/>
@@ -1438,28 +1438,28 @@
         <v>Enter Data in 'Date of Expense' &amp; 'Currency Amount' as Needed</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="11"/>
       <c r="B56" s="13"/>
       <c r="C56" s="14"/>
       <c r="D56" s="11"/>
       <c r="E56" s="16"/>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="11"/>
       <c r="B57" s="13"/>
       <c r="C57" s="14"/>
       <c r="D57" s="11"/>
       <c r="E57" s="16"/>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="11"/>
       <c r="B58" s="13"/>
       <c r="C58" s="14"/>
       <c r="D58" s="11"/>
       <c r="E58" s="16"/>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="11"/>
       <c r="B59" s="13"/>
       <c r="C59" s="14"/>

</xml_diff>